<commit_message>
Update initial burndown chart
</commit_message>
<xml_diff>
--- a/Initial burndown Chart.xlsx
+++ b/Initial burndown Chart.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24740" windowHeight="15620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Initial Burn Down Chart for Team 17</t>
   </si>
@@ -52,6 +57,45 @@
   </si>
   <si>
     <t>03-04-2013 (First meeting)</t>
+  </si>
+  <si>
+    <t>03-06-2013()</t>
+  </si>
+  <si>
+    <t>03-08-2013()</t>
+  </si>
+  <si>
+    <t>03-11-2013()</t>
+  </si>
+  <si>
+    <t>03-13-2013()</t>
+  </si>
+  <si>
+    <t>03-15-2013()</t>
+  </si>
+  <si>
+    <t>03-18-2013()</t>
+  </si>
+  <si>
+    <t>03-20-2013()</t>
+  </si>
+  <si>
+    <t>03-22-2013()</t>
+  </si>
+  <si>
+    <t>03-25-2013()</t>
+  </si>
+  <si>
+    <t>03-27-2013()</t>
+  </si>
+  <si>
+    <t>03-29-2013()</t>
+  </si>
+  <si>
+    <t>04-01-2013()</t>
+  </si>
+  <si>
+    <t>04-02-2013(Fianl Deadline)</t>
   </si>
 </sst>
 </file>
@@ -102,10 +146,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,16 +208,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>20</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -187,8 +226,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="7961216"/>
-        <c:axId val="7971200"/>
+        <c:axId val="518780440"/>
+        <c:axId val="114241688"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -214,19 +253,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>57.75</c:v>
+                  <c:v>61.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>60.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>55.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>50.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -254,49 +323,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>57.75</c:v>
+                  <c:v>61.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>60.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -313,11 +343,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="7961216"/>
-        <c:axId val="7971200"/>
+        <c:axId val="518780440"/>
+        <c:axId val="114241688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7961216"/>
+        <c:axId val="518780440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -327,7 +357,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="7971200"/>
+        <c:crossAx val="114241688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -336,7 +366,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7971200"/>
+        <c:axId val="114241688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -347,8 +377,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="7961216"/>
-        <c:crossesAt val="1"/>
+        <c:crossAx val="518780440"/>
+        <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -694,23 +724,23 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="4" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -727,7 +757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>0</v>
       </c>
@@ -735,180 +765,211 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>57.75</v>
+        <v>61.75</v>
       </c>
       <c r="D4">
-        <v>57.75</v>
+        <v>61.75</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="C5">
-        <v>55</v>
+        <f>A25-1.5</f>
+        <v>60.25</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <f>A25-B5</f>
+        <v>60.25</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
       <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>55.25</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="C7">
-        <v>45</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50.25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>45.25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>25</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>11</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>12</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>13</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>14</v>
       </c>
-      <c r="B18">
-        <v>20</v>
-      </c>
       <c r="C18">
         <v>0</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25">
-        <v>57.75</v>
+        <v>61.75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -918,9 +979,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -930,8 +996,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>